<commit_message>
Merge ScanMe card back into mobster pitch
</commit_message>
<xml_diff>
--- a/Logbook.xlsx
+++ b/Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Blindesigners\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDFE039-ABFD-4476-BC7C-23823F528B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63889D8F-02BC-42D8-812E-640227A88122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16068" yWindow="7680" windowWidth="16764" windowHeight="12204" activeTab="1" xr2:uid="{2DABE83D-9220-4142-A5E3-92CC56B15272}"/>
+    <workbookView xWindow="12312" yWindow="7416" windowWidth="30960" windowHeight="12204" activeTab="1" xr2:uid="{2DABE83D-9220-4142-A5E3-92CC56B15272}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Payment ID</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>DWK</t>
-  </si>
-  <si>
     <t>$DorkyDomains</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>$rebeccakayknight</t>
   </si>
   <si>
-    <t>Isaac</t>
-  </si>
-  <si>
     <t>Dan Velvet</t>
   </si>
   <si>
@@ -109,6 +103,15 @@
   </si>
   <si>
     <t>Free</t>
+  </si>
+  <si>
+    <t>Rocko</t>
+  </si>
+  <si>
+    <t>Ponzi</t>
+  </si>
+  <si>
+    <t>CashApp</t>
   </si>
 </sst>
 </file>
@@ -484,14 +487,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0266BDDC-B7E1-4EA9-A989-F9C46A3429BC}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" customWidth="1"/>
@@ -500,16 +504,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -517,52 +521,66 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -572,10 +590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AA820D-6CD4-4385-B2F7-DBB51C166D9A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,70 +604,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>